<commit_message>
Changed date of sample flight
</commit_message>
<xml_diff>
--- a/autoflpy/data/Checklists_emergency.xlsx
+++ b/autoflpy/data/Checklists_emergency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aw6g15\University of Southampton\Adrian Weishaeupl - Documents\PhD\2019\AutoFLpy\AutoFLpy\autoflpy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="6_{FD448723-9E88-4AEF-9B19-2759A1E39832}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{473185F7-2442-4E2C-AAB5-F16B618F7037}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="6_{FD448723-9E88-4AEF-9B19-2759A1E39832}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{07E0ACD2-1ADA-46BF-AE65-103A69F71CCE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form1" sheetId="1" r:id="rId1"/>
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>43466.65121527778</v>
+        <v>43475.65121527778</v>
       </c>
       <c r="C2" s="3">
         <v>43466.651828703703</v>
@@ -684,17 +684,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="4de5569b-e040-4e3a-896c-3d10ceee17bb">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -901,27 +896,23 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="4de5569b-e040-4e3a-896c-3d10ceee17bb">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC263F84-3C12-4CB9-B561-E45814456A2D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C58D8165-7001-47E2-B2DB-E33FECDA23E8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="4de5569b-e040-4e3a-896c-3d10ceee17bb"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d6e80eea-1699-4de5-969f-0d9eb2724e77"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -946,9 +937,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C58D8165-7001-47E2-B2DB-E33FECDA23E8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC263F84-3C12-4CB9-B561-E45814456A2D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4de5569b-e040-4e3a-896c-3d10ceee17bb"/>
+    <ds:schemaRef ds:uri="d6e80eea-1699-4de5-969f-0d9eb2724e77"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Checklist name bug fixed
</commit_message>
<xml_diff>
--- a/autoflpy/data/Checklists_emergency.xlsx
+++ b/autoflpy/data/Checklists_emergency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aw6g15\University of Southampton\Adrian Weishaeupl - Documents\PhD\2019\AutoFLpy\AutoFLpy\autoflpy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="6_{FD448723-9E88-4AEF-9B19-2759A1E39832}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{07E0ACD2-1ADA-46BF-AE65-103A69F71CCE}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="6_{FD448723-9E88-4AEF-9B19-2759A1E39832}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{623BEA0F-3502-4036-91E7-A6947C35D3EF}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>Start time</t>
   </si>
   <si>
-    <t>Completion time</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>v0.2</t>
+  </si>
+  <si>
+    <t>End time</t>
   </si>
 </sst>
 </file>
@@ -206,7 +206,7 @@
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Completion time" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="End time" dataDxfId="9"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="7"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Emergency Checklist" dataDxfId="6"/>
@@ -521,7 +521,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,34 +537,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -578,31 +578,31 @@
         <v>43466.651828703703</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="J2" s="1">
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -616,31 +616,31 @@
         <v>43759.654803240701</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -664,17 +664,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -684,15 +684,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010045D28EA33B1D374F90B741F2AF73533E" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="70f0338854bc56f50ac4daf9a6be0e17">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d6e80eea-1699-4de5-969f-0d9eb2724e77" xmlns:ns3="4de5569b-e040-4e3a-896c-3d10ceee17bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88fb165263e20f462f96975fe477339d" ns2:_="" ns3:_="">
     <xsd:import namespace="d6e80eea-1699-4de5-969f-0d9eb2724e77"/>
@@ -895,6 +886,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -910,14 +910,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C58D8165-7001-47E2-B2DB-E33FECDA23E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD52C885-CCBC-4993-BEC0-35EBEB3D3CAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -936,6 +928,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C58D8165-7001-47E2-B2DB-E33FECDA23E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC263F84-3C12-4CB9-B561-E45814456A2D}">
   <ds:schemaRefs>

</xml_diff>